<commit_message>
gst and other fields added
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -432,8 +432,8 @@
       <c r="A2" t="str">
         <v>52.45</v>
       </c>
-      <c r="B2" t="str">
-        <v>99</v>
+      <c r="B2">
+        <v>98</v>
       </c>
       <c r="C2" t="str">
         <v>Backpack</v>
@@ -450,8 +450,8 @@
       <c r="G2">
         <v>10</v>
       </c>
-      <c r="H2">
-        <v>2</v>
+      <c r="H2" t="str">
+        <v>5</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
search bar functionality added
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,149 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sansk\Downloads\cartapp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AD0565-2AE0-4006-A8D1-E941A500A670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Stock" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>quantity</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>company</t>
-  </si>
-  <si>
-    <t>expiry</t>
-  </si>
-  <si>
-    <t>batch</t>
-  </si>
-  <si>
-    <t>packsize</t>
-  </si>
-  <si>
-    <t>gst</t>
-  </si>
-  <si>
-    <t>52.45</t>
-  </si>
-  <si>
-    <t>Backpack</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>Indiana Design Tshirt</t>
-  </si>
-  <si>
-    <t>xyz</t>
-  </si>
-  <si>
-    <t>13.90</t>
-  </si>
-  <si>
-    <t>Black Clipped Tshirt</t>
-  </si>
-  <si>
-    <t>68.35</t>
-  </si>
-  <si>
-    <t>Alder Light 2 Tones</t>
-  </si>
-  <si>
-    <t>52.84</t>
-  </si>
-  <si>
-    <t>Backpack Mohave Gold" Season</t>
-  </si>
-  <si>
-    <t>Element Tshirt</t>
-  </si>
-  <si>
-    <t>168.75</t>
-  </si>
-  <si>
-    <t>Heavy Puff TW Chaqueta</t>
-  </si>
-  <si>
-    <t>47.50</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hombre Mid Grey Tshirt</t>
-  </si>
-  <si>
-    <t>64.94</t>
-  </si>
-  <si>
-    <t>Sweat Shirt</t>
-  </si>
-  <si>
-    <t>29.84</t>
-  </si>
-  <si>
-    <t>Camiseta Tshirt Signature</t>
-  </si>
-  <si>
-    <t>99.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scateboard Pre-Built Complete </t>
-  </si>
-  <si>
-    <t>27.06</t>
-  </si>
-  <si>
-    <t>Grey Printed Tshirt</t>
-  </si>
-  <si>
-    <t>86.52</t>
-  </si>
-  <si>
-    <t>Alder Light Olive</t>
-  </si>
-  <si>
-    <t>73.50</t>
-  </si>
-  <si>
-    <t>Puff TW Negro Jacket</t>
-  </si>
-  <si>
-    <t>serial</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -180,14 +72,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -512,59 +396,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1">
+      <c r="A1" t="str">
+        <v>serial</v>
+      </c>
+      <c r="B1" t="str">
+        <v>price</v>
+      </c>
+      <c r="C1" t="str">
+        <v>quantity</v>
+      </c>
+      <c r="D1" t="str">
+        <v>title</v>
+      </c>
+      <c r="E1" t="str">
+        <v>company</v>
+      </c>
+      <c r="F1" t="str">
+        <v>expiry</v>
+      </c>
+      <c r="G1" t="str">
+        <v>batch</v>
+      </c>
+      <c r="H1" t="str">
+        <v>packsize</v>
+      </c>
+      <c r="I1" t="str">
+        <v>gst</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
+      <c r="B2" t="str">
+        <v>52.45</v>
       </c>
       <c r="C2">
         <v>98</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
+      <c r="D2" t="str">
+        <v>Backpa</v>
+      </c>
+      <c r="E2" t="str">
+        <v>abcd</v>
       </c>
       <c r="F2">
         <v>44727</v>
@@ -575,25 +456,25 @@
       <c r="H2">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I2" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>12</v>
+      <c r="B3" t="str">
+        <v>18</v>
       </c>
       <c r="C3">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
+      <c r="D3" t="str">
+        <v>Indiana  Tshirt</v>
+      </c>
+      <c r="E3" t="str">
+        <v>xyz</v>
       </c>
       <c r="F3">
         <v>44728</v>
@@ -608,21 +489,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
+      <c r="B4" t="str">
+        <v>13.90</v>
       </c>
       <c r="C4">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
+      <c r="D4" t="str">
+        <v>Back Clipped Tshirt</v>
+      </c>
+      <c r="E4" t="str">
+        <v>abc</v>
       </c>
       <c r="F4">
         <v>44729</v>
@@ -637,21 +518,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
+      <c r="B5" t="str">
+        <v>68.35</v>
       </c>
       <c r="C5">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
+      <c r="D5" t="str">
+        <v>Alder Light 2 Tones</v>
+      </c>
+      <c r="E5" t="str">
+        <v>abc</v>
       </c>
       <c r="F5">
         <v>44730</v>
@@ -666,21 +547,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>19</v>
+      <c r="B6" t="str">
+        <v>52.84</v>
       </c>
       <c r="C6">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
+      <c r="D6" t="str">
+        <v>Backpack Mohave Gold" Season</v>
+      </c>
+      <c r="E6" t="str">
+        <v>abc</v>
       </c>
       <c r="F6">
         <v>44731</v>
@@ -695,21 +576,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>15</v>
+      <c r="B7" t="str">
+        <v>13.90</v>
       </c>
       <c r="C7">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
+      <c r="D7" t="str">
+        <v>Element Tshirt</v>
+      </c>
+      <c r="E7" t="str">
+        <v>abc</v>
       </c>
       <c r="F7">
         <v>44732</v>
@@ -724,21 +605,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>22</v>
+      <c r="B8" t="str">
+        <v>168.75</v>
       </c>
       <c r="C8">
         <v>10</v>
       </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
+      <c r="D8" t="str">
+        <v>Heavy Puff TW Chaqueta</v>
+      </c>
+      <c r="E8" t="str">
+        <v>abc</v>
       </c>
       <c r="F8">
         <v>44733</v>
@@ -753,21 +634,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>24</v>
+      <c r="B9" t="str">
+        <v>47.50</v>
       </c>
       <c r="C9">
         <v>10</v>
       </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
+      <c r="D9" t="str">
+        <v xml:space="preserve"> Hombre Mid Grey Tshirt</v>
+      </c>
+      <c r="E9" t="str">
+        <v>abc</v>
       </c>
       <c r="F9">
         <v>44734</v>
@@ -782,21 +663,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>26</v>
+      <c r="B10" t="str">
+        <v>64.94</v>
       </c>
       <c r="C10">
         <v>10</v>
       </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s">
-        <v>10</v>
+      <c r="D10" t="str">
+        <v>Sweat Shirt</v>
+      </c>
+      <c r="E10" t="str">
+        <v>abc</v>
       </c>
       <c r="F10">
         <v>44735</v>
@@ -811,21 +692,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>28</v>
+      <c r="B11" t="str">
+        <v>29.84</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
-      <c r="D11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" t="s">
-        <v>10</v>
+      <c r="D11" t="str">
+        <v>Camiseta Tshirt Signature</v>
+      </c>
+      <c r="E11" t="str">
+        <v>abc</v>
       </c>
       <c r="F11">
         <v>44736</v>
@@ -840,21 +721,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>30</v>
+      <c r="B12" t="str">
+        <v>99.00</v>
       </c>
       <c r="C12">
         <v>10</v>
       </c>
-      <c r="D12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" t="s">
-        <v>10</v>
+      <c r="D12" t="str">
+        <v xml:space="preserve">Scateboard Pre-Built Complete </v>
+      </c>
+      <c r="E12" t="str">
+        <v>abc</v>
       </c>
       <c r="F12">
         <v>44737</v>
@@ -869,21 +750,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>32</v>
+      <c r="B13" t="str">
+        <v>27.06</v>
       </c>
       <c r="C13">
         <v>10</v>
       </c>
-      <c r="D13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" t="s">
-        <v>10</v>
+      <c r="D13" t="str">
+        <v>Grey Printed Tshirt</v>
+      </c>
+      <c r="E13" t="str">
+        <v>abc</v>
       </c>
       <c r="F13">
         <v>44738</v>
@@ -898,21 +779,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>34</v>
+      <c r="B14" t="str">
+        <v>86.52</v>
       </c>
       <c r="C14">
         <v>10</v>
       </c>
-      <c r="D14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" t="s">
-        <v>10</v>
+      <c r="D14" t="str">
+        <v>Alder Light Olive</v>
+      </c>
+      <c r="E14" t="str">
+        <v>abc</v>
       </c>
       <c r="F14">
         <v>44739</v>
@@ -927,21 +808,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>36</v>
+      <c r="B15" t="str">
+        <v>73.50</v>
       </c>
       <c r="C15">
         <v>10</v>
       </c>
-      <c r="D15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" t="s">
-        <v>10</v>
+      <c r="D15" t="str">
+        <v>Puff TW Negro Jacket</v>
+      </c>
+      <c r="E15" t="str">
+        <v>abc</v>
       </c>
       <c r="F15">
         <v>44740</v>
@@ -957,10 +838,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B1:I15" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I15"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
billing to be fixed
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -439,10 +439,10 @@
         <v>52.45</v>
       </c>
       <c r="C2">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D2" t="str">
-        <v>Backpa</v>
+        <v>Backpack</v>
       </c>
       <c r="E2" t="str">
         <v>abcd</v>
@@ -468,7 +468,7 @@
         <v>18</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" t="str">
         <v>Indiana  Tshirt</v>
@@ -497,7 +497,7 @@
         <v>13.90</v>
       </c>
       <c r="C4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" t="str">
         <v>Back Clipped Tshirt</v>

</xml_diff>